<commit_message>
Added additional columns to project summary report
</commit_message>
<xml_diff>
--- a/projects2/static/projects2/projects_summary_template.xlsx
+++ b/projects2/static/projects2/projects_summary_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Section</t>
   </si>
   <si>
-    <t>Project Overview</t>
-  </si>
-  <si>
     <t>Activity Type</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Completed List of Funding Sources</t>
   </si>
   <si>
-    <t>Project Leads</t>
-  </si>
-  <si>
     <t>Tags / Keywords</t>
   </si>
   <si>
@@ -71,7 +65,73 @@
     <t>Metadata</t>
   </si>
   <si>
-    <t>Project Title</t>
+    <t>Special Equipment?</t>
+  </si>
+  <si>
+    <t>Field Component?</t>
+  </si>
+  <si>
+    <t>Data Collected or Generated?</t>
+  </si>
+  <si>
+    <t>Data Products</t>
+  </si>
+  <si>
+    <t>Type of Data</t>
+  </si>
+  <si>
+    <t>Data Management</t>
+  </si>
+  <si>
+    <t>Labortory Work?</t>
+  </si>
+  <si>
+    <t>Special IT Requirements</t>
+  </si>
+  <si>
+    <t>Additional Notes</t>
+  </si>
+  <si>
+    <t>Financial Coding</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>Year Specific Overview</t>
+  </si>
+  <si>
+    <t>A-Base</t>
+  </si>
+  <si>
+    <t>B-Base</t>
+  </si>
+  <si>
+    <t>C-Base</t>
+  </si>
+  <si>
+    <t>O&amp;M Costs Totals</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Priorities</t>
+  </si>
+  <si>
+    <t>Project General Overview</t>
   </si>
 </sst>
 </file>
@@ -79,9 +139,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +164,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -131,15 +205,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -422,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -446,59 +524,171 @@
     <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="5" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:35" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="R1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AF1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+    </row>
+    <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
+      <c r="V2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="R1:AD1"/>
+    <mergeCell ref="AF1:AI1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>